<commit_message>
update case files and templates to 2025
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B304001C-F00C-427F-96C2-32D45E3A16A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0975DF3B-3414-4224-9F15-F7ADBDCECB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="12690" windowWidth="13965" windowHeight="15585" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -420,10 +420,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B2" s="1">
         <v>100000</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B3" s="1">
         <v>100000</v>
@@ -503,12 +503,11 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B4" s="1">
         <v>100000</v>
@@ -525,7 +524,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -540,7 +539,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -553,7 +552,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -566,7 +565,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -579,7 +578,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -592,7 +591,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -605,7 +604,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -618,7 +617,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -631,7 +630,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -644,7 +643,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -657,7 +656,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -670,7 +669,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -683,7 +682,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -696,7 +695,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -709,7 +708,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -722,7 +721,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -735,7 +734,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -748,7 +747,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -761,7 +760,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -774,7 +773,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -787,7 +786,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -800,7 +799,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -813,7 +812,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -826,7 +825,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -839,7 +838,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -852,7 +851,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -865,7 +864,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -878,19 +877,6 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2054</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
         <v>2055</v>
       </c>
     </row>
@@ -902,10 +888,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +938,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B2" s="1">
         <v>80000</v>
@@ -967,7 +953,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B3" s="1">
         <v>80000</v>
@@ -982,7 +968,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B4" s="1">
         <v>85000</v>
@@ -997,7 +983,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1010,7 +996,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1023,7 +1009,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1036,7 +1022,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1049,7 +1035,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1062,7 +1048,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1075,7 +1061,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1088,7 +1074,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1101,7 +1087,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1114,7 +1100,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1127,7 +1113,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1140,7 +1126,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1153,7 +1139,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1166,7 +1152,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1179,7 +1165,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1192,7 +1178,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1205,7 +1191,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1218,7 +1204,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1231,7 +1217,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1244,7 +1230,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1257,7 +1243,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1270,7 +1256,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1283,7 +1269,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1296,7 +1282,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1309,7 +1295,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1322,7 +1308,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1335,7 +1321,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1348,7 +1334,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1361,7 +1347,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1374,24 +1360,11 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2056</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+        <v>2057</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36">
         <v>2058</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change wage&contrib column names for consistency
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0975DF3B-3414-4224-9F15-F7ADBDCECB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A295070-C45F-446F-97F6-D3E258D0BA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="10690" yWindow="7090" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -42,28 +42,28 @@
     <t>year</t>
   </si>
   <si>
-    <t>Roth X</t>
-  </si>
-  <si>
-    <t>ctrb taxable</t>
-  </si>
-  <si>
-    <t>ctrb 401k</t>
-  </si>
-  <si>
-    <t>ctrb Roth 401k</t>
-  </si>
-  <si>
-    <t>ctrb IRA</t>
-  </si>
-  <si>
-    <t>ctrb Roth IRA</t>
-  </si>
-  <si>
     <t>anticipated wages</t>
   </si>
   <si>
     <t>big-ticket items</t>
+  </si>
+  <si>
+    <t>Roth conv</t>
+  </si>
+  <si>
+    <t>taxable ctrb</t>
+  </si>
+  <si>
+    <t>401k ctrb</t>
+  </si>
+  <si>
+    <t>Roth 401k ctrb</t>
+  </si>
+  <si>
+    <t>IRA ctrb</t>
+  </si>
+  <si>
+    <t>Roth IRA ctrb</t>
   </si>
 </sst>
 </file>
@@ -73,13 +73,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +431,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,32 +452,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -891,7 +899,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,32 +916,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add NIIT - simplify quick start
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A295070-C45F-446F-97F6-D3E258D0BA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64A8F46-BCD3-4A85-BE4A-4B5800FAC2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10690" yWindow="7090" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="345" yWindow="8055" windowWidth="15045" windowHeight="11700" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +84,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,10 +116,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +439,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,90 +492,93 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>100000</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
-        <v>15000</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="A2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
+        <v>6500</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2026</v>
-      </c>
-      <c r="B3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
-        <v>15000</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4">
+        <v>6500</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2027</v>
-      </c>
-      <c r="B4" s="1">
-        <v>100000</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1">
-        <v>50000</v>
-      </c>
-      <c r="I4" s="1"/>
+      <c r="A4" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
+        <v>7000</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2028</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
-        <v>50000</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="A5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4">
+        <v>7000</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2029</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="A6" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>7000</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <v>20000</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2030</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100000</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>15000</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -573,11 +587,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2031</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>2026</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100000</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>15000</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -586,20 +604,24 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2032</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>2027</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100000</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>50000</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2033</v>
+        <v>2028</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -607,12 +629,14 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1">
+        <v>50000</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2034</v>
+        <v>2029</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -625,7 +649,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -638,7 +662,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2036</v>
+        <v>2031</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -651,7 +675,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2037</v>
+        <v>2032</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -664,7 +688,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2038</v>
+        <v>2033</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -677,7 +701,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2039</v>
+        <v>2034</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -690,7 +714,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -703,7 +727,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2041</v>
+        <v>2036</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -716,7 +740,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2042</v>
+        <v>2037</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -729,7 +753,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2043</v>
+        <v>2038</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -742,7 +766,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2044</v>
+        <v>2039</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -755,7 +779,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -768,7 +792,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -781,7 +805,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -794,7 +818,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2048</v>
+        <v>2043</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -807,7 +831,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2049</v>
+        <v>2044</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -820,7 +844,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -833,7 +857,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2051</v>
+        <v>2046</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -846,7 +870,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2052</v>
+        <v>2047</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -859,7 +883,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2053</v>
+        <v>2048</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -872,7 +896,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2054</v>
+        <v>2049</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -885,6 +909,71 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>2050</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2051</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2052</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2053</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2054</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>2055</v>
       </c>
     </row>
@@ -896,10 +985,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,222 +1034,234 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>80000</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="A2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2026</v>
-      </c>
-      <c r="B3" s="1">
-        <v>80000</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2027</v>
-      </c>
-      <c r="B4" s="1">
-        <v>85000</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="A4" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
+        <v>4000</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2028</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>12000</v>
+      </c>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2029</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="A6" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2030</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+        <v>2025</v>
+      </c>
+      <c r="B7" s="6">
+        <v>80000</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2031</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>2025</v>
+      </c>
+      <c r="B8" s="6">
+        <v>80000</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2032</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+        <v>2026</v>
+      </c>
+      <c r="B9" s="6">
+        <v>80000</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2033</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+        <v>2027</v>
+      </c>
+      <c r="B10" s="6">
+        <v>85000</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2034</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+        <v>2028</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2035</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+        <v>2029</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2036</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+        <v>2030</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2037</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+        <v>2031</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2038</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>2032</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2039</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+        <v>2033</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2040</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>2034</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2041</v>
+        <v>2035</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1173,7 +1274,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2042</v>
+        <v>2036</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1186,7 +1287,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2043</v>
+        <v>2037</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1199,7 +1300,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2044</v>
+        <v>2038</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1212,7 +1313,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2045</v>
+        <v>2039</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1225,7 +1326,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2046</v>
+        <v>2040</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1238,7 +1339,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2047</v>
+        <v>2041</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1251,7 +1352,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2048</v>
+        <v>2042</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1264,7 +1365,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2049</v>
+        <v>2043</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1277,7 +1378,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2050</v>
+        <v>2044</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1290,7 +1391,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2051</v>
+        <v>2045</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1303,7 +1404,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2052</v>
+        <v>2046</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1316,7 +1417,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2053</v>
+        <v>2047</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1329,7 +1430,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2054</v>
+        <v>2048</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1342,7 +1443,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2055</v>
+        <v>2049</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1355,7 +1456,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2056</v>
+        <v>2050</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1368,11 +1469,89 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2057</v>
-      </c>
+        <v>2051</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>2052</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2053</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2054</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2055</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2056</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>2058</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Few fixes/improvements and kick version
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64A8F46-BCD3-4A85-BE4A-4B5800FAC2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E27C23-E62D-4D8C-BE43-5B2A6AE98967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="8055" windowWidth="15045" windowHeight="11700" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -985,10 +985,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B8" s="6">
         <v>80000</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B9" s="6">
-        <v>80000</v>
+        <v>85000</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1155,11 +1155,9 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2027</v>
-      </c>
-      <c r="B10" s="6">
-        <v>85000</v>
-      </c>
+        <v>2028</v>
+      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1170,7 +1168,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1183,7 +1181,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1196,7 +1194,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1209,7 +1207,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1222,7 +1220,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1235,7 +1233,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1248,20 +1246,20 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2034</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+        <v>2035</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1274,7 +1272,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1287,7 +1285,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1300,7 +1298,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1313,7 +1311,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1326,7 +1324,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1339,7 +1337,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1352,7 +1350,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1365,7 +1363,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1378,7 +1376,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1391,7 +1389,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1404,7 +1402,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1417,7 +1415,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1430,7 +1428,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1443,7 +1441,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1456,7 +1454,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1469,7 +1467,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1482,7 +1480,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1495,7 +1493,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1508,7 +1506,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1521,7 +1519,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1534,24 +1532,11 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2056</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+        <v>2057</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
         <v>2058</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement I/O on Household Financial Profile
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E27C23-E62D-4D8C-BE43-5B2A6AE98967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0235C7D1-BCBA-44E8-8527-87A84E08C555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
     <sheet name="Jill" sheetId="2" r:id="rId2"/>
+    <sheet name="Debts" sheetId="3" r:id="rId3"/>
+    <sheet name="Fixed Assets" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>year</t>
   </si>
@@ -64,6 +66,39 @@
   </si>
   <si>
     <t>Roth IRA ctrb</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>basis</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>yod</t>
+  </si>
+  <si>
+    <t>commission</t>
+  </si>
+  <si>
+    <t>PR mortgage</t>
+  </si>
+  <si>
+    <t>house</t>
   </si>
 </sst>
 </file>
@@ -74,7 +109,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +129,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -124,6 +167,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,7 +1032,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -1543,4 +1588,110 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA707BF-A4A7-4841-BFD6-9B94FB900DD0}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1">
+        <v>250000</v>
+      </c>
+      <c r="F2">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First working version addressing issue #22 (Dale's)
</commit_message>
<xml_diff>
--- a/examples/jack+jill.xlsx
+++ b/examples/jack+jill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0235C7D1-BCBA-44E8-8527-87A84E08C555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C095B-2637-4002-8A66-C4C993C6A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>year</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>commission</t>
-  </si>
-  <si>
-    <t>PR mortgage</t>
-  </si>
-  <si>
-    <t>house</t>
   </si>
 </sst>
 </file>
@@ -1592,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA707BF-A4A7-4841-BFD6-9B94FB900DD0}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,26 +1623,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>2000</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
-        <v>250000</v>
-      </c>
-      <c r="F2">
-        <v>3.5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1658,13 +1632,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1675,7 +1652,7 @@
       <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="8" t="s">

</xml_diff>